<commit_message>
prints feature importance based on csv data
</commit_message>
<xml_diff>
--- a/profiles_matched.xlsx
+++ b/profiles_matched.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,30 +525,30 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>418</v>
+        <v>350</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.73</t>
+          <t>0.68</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Liked by you &amp;</t>
+          <t>&amp;</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -562,7 +562,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>QMU</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -583,17 +583,17 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>£913-£1602</t>
+          <t>£919-£1785</t>
         </is>
       </c>
     </row>
@@ -602,16 +602,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jane Johnson</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.68</t>
+          <t>0.64</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -621,11 +621,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -634,17 +634,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>KCL</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Business</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -660,7 +660,7 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>£805-£1668</t>
+          <t>£922-£1056</t>
         </is>
       </c>
     </row>
@@ -679,16 +679,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.64</t>
+          <t>0.63</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -698,15 +698,15 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -716,12 +716,12 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>UCL</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -742,12 +742,12 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>£922-£1056</t>
+          <t>£665-£1082</t>
         </is>
       </c>
     </row>
@@ -756,34 +756,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>309</v>
+        <v>460</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Alice Williams</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.63</t>
+          <t>0.60</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>&amp;</t>
+          <t>&amp; Liked you</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -793,38 +793,38 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>UCL</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
+          <t>QMU</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>£665-£1082</t>
+          <t>£583-£916</t>
         </is>
       </c>
     </row>
@@ -833,11 +833,11 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>460</v>
+        <v>268</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>Jane Smith</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -847,16 +847,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Liked by you &amp;</t>
+          <t>&amp;</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -865,25 +865,21 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Both</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>QMU</t>
+          <t>KCL</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
+          <t>Cruising</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -896,12 +892,12 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>£583-£916</t>
+          <t>£440-£1858</t>
         </is>
       </c>
     </row>
@@ -910,16 +906,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>268</v>
+        <v>134</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jane Smith</t>
+          <t>Bob Doe</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.60</t>
+          <t>0.57</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -929,11 +925,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -942,12 +938,12 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>none</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
@@ -957,11 +953,7 @@
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
           <t>Night</t>
@@ -969,12 +961,12 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>£440-£1858</t>
+          <t>£881-£1713</t>
         </is>
       </c>
     </row>
@@ -983,26 +975,26 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>134</v>
+        <v>192</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Bob Doe</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>0.55</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>&amp;</t>
+          <t>Liked by you &amp;</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -1010,27 +1002,35 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Both</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>none</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
+          <t>QMU</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="O8" t="inlineStr">
         <is>
           <t>Night</t>
@@ -1043,7 +1043,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>£881-£1713</t>
+          <t>£459-£1836</t>
         </is>
       </c>
     </row>
@@ -1052,11 +1052,11 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>John Johnson</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1071,15 +1071,15 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1089,38 +1089,30 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>QMU</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
+          <t>UCL</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>£459-£1836</t>
+          <t>£805-£1027</t>
         </is>
       </c>
     </row>
@@ -1129,11 +1121,11 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>201</v>
+        <v>257</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>John Johnson</t>
+          <t>Jane Williams</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1148,11 +1140,11 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1161,22 +1153,30 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>City</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="O10" t="inlineStr">
         <is>
           <t>Morning</t>
@@ -1184,12 +1184,12 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>£805-£1027</t>
+          <t>£716-£974</t>
         </is>
       </c>
     </row>
@@ -1198,16 +1198,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>257</v>
+        <v>175</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Jane Williams</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.55</t>
+          <t>0.49</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1217,15 +1217,15 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1235,38 +1235,38 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr"/>
+          <t>UCL</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
+          <t>Student</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>£716-£974</t>
+          <t>£469-£1154</t>
         </is>
       </c>
     </row>
@@ -1275,7 +1275,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>125</v>
+        <v>301</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.47</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1294,56 +1294,52 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Computer Science</t>
-        </is>
-      </c>
+          <t>UCL</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>£872-£1129</t>
+          <t>£889-£1554</t>
         </is>
       </c>
     </row>
@@ -1352,34 +1348,34 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>175</v>
+        <v>428</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.49</t>
+          <t>0.46</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>&amp;</t>
+          <t>&amp; Liked you</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1389,17 +1385,13 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>UCL</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
+          <t>KCL</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="M13" t="inlineStr"/>
@@ -1410,17 +1402,17 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>£469-£1154</t>
+          <t>£783-£977</t>
         </is>
       </c>
     </row>
@@ -1429,58 +1421,58 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>301</v>
+        <v>488</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Alice Doe</t>
+          <t>Bob Johnson</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.47</t>
+          <t>0.44</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>&amp;</t>
+          <t>Liked by you &amp; Liked you</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Both</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>UCL</t>
+          <t>KCL</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
           <t>Night</t>
@@ -1488,12 +1480,12 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>£889-£1554</t>
+          <t>£300-£1798</t>
         </is>
       </c>
     </row>
@@ -1502,26 +1494,26 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>428</v>
+        <v>335</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Alice Johnson</t>
+          <t>John Smith</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.46</t>
+          <t>0.41</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Liked by you &amp;</t>
+          <t>&amp;</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1529,44 +1521,44 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Both</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>KCL</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr"/>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Cruising</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>UK</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>£783-£977</t>
+          <t>£920-£1944</t>
         </is>
       </c>
     </row>
@@ -1575,44 +1567,44 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>488</v>
+        <v>206</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.44</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Liked by you &amp; Liked you</t>
+          <t>&amp;</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>KCL</t>
+          <t>City</t>
         </is>
       </c>
       <c r="K16" t="inlineStr"/>
@@ -1626,20 +1618,24 @@
           <t>Tech</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>£300-£1798</t>
+          <t>£688-£1536</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1644,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>335</v>
+        <v>123</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1657,7 +1653,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.41</t>
+          <t>0.39</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1667,11 +1663,11 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1685,21 +1681,21 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
+          <t>QMU</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="O17" t="inlineStr">
         <is>
           <t>Night</t>
@@ -1707,12 +1703,12 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>UK</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>£920-£1944</t>
+          <t>£418-£1719</t>
         </is>
       </c>
     </row>
@@ -1721,30 +1717,30 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>206</v>
+        <v>380</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>John Doe</t>
+          <t>Alice Johnson</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>&amp;</t>
+          <t>Liked by you &amp; Liked you</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1753,7 +1749,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Both</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1769,27 +1765,27 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>Tech</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Night</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>£688-£1536</t>
+          <t>£976-£1191</t>
         </is>
       </c>
     </row>
@@ -1798,16 +1794,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>123</v>
+        <v>193</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>John Smith</t>
+          <t>Jane Doe</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.39</t>
+          <t>0.35</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1817,11 +1813,11 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1830,29 +1826,29 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Both</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>QMU</t>
+          <t>none</t>
         </is>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+          <t>Working</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>Tech</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Night</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1862,7 +1858,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>£418-£1719</t>
+          <t>£415-£891</t>
         </is>
       </c>
     </row>
@@ -1871,30 +1867,30 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>246</v>
+        <v>90</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
+          <t>John Williams</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.38</t>
+          <t>0.26</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>&amp;</t>
+          <t>Liked by you &amp;</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Block 3, first 5</t>
+          <t>Block 2, last 5</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1908,23 +1904,19 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>QMU</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
+          <t>City</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Student</t>
+          <t>Cruising</t>
         </is>
       </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -1938,302 +1930,6 @@
         </is>
       </c>
       <c r="Q20" t="inlineStr">
-        <is>
-          <t>£983-£1978</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>380</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alice Johnson</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Liked by you &amp;</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Block 3, first 5</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>22</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Both</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Finance</t>
-        </is>
-      </c>
-      <c r="N21" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>Night</t>
-        </is>
-      </c>
-      <c r="P21" t="inlineStr">
-        <is>
-          <t>Australia</t>
-        </is>
-      </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>£976-£1191</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" t="n">
-        <v>193</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Jane Doe</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>&amp;</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Block 3, first 5</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
-        <v>24</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr"/>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>Working</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Tech</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>£415-£891</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" t="n">
-        <v>107</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Bob Doe</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>0.32</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>&amp;</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Block 3, first 5</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
-        <v>26</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Both</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>QMU</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>Student</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="P23" t="inlineStr">
-        <is>
-          <t>UK</t>
-        </is>
-      </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>£951-£1669</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" t="n">
-        <v>90</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>John Williams</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>0.26</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>&amp;</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Block 3, first 5</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>19</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>City</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Cruising</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr"/>
-      <c r="N24" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="P24" t="inlineStr">
-        <is>
-          <t>USA</t>
-        </is>
-      </c>
-      <c r="Q24" t="inlineStr">
         <is>
           <t>£926-£1039</t>
         </is>

</xml_diff>